<commit_message>
Añadiendo lectura de S3
</commit_message>
<xml_diff>
--- a/email_triage/Actividades.xlsx
+++ b/email_triage/Actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanfiel91\Documents\Repositories\Work\MarcosArquitecturaPersonal\vimotions-booking-automation-lambda\email_triage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanfiel91\Documents\Repositories\Work\Last_Stage_Vim\vimotions-booking-automation-lambda\email_triage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CE4B55-304E-4329-9912-4C86050E0597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184B6BAB-7132-4C87-A1C7-AF12B746471F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11310" yWindow="1500" windowWidth="22035" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="1920" windowWidth="20115" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="168">
   <si>
     <t>Nombre</t>
   </si>
@@ -513,9 +513,6 @@
     <t>Entrada al zoo Cocodrilo Park en Agüimes</t>
   </si>
   <si>
-    <t>"Buenas, Date of the activity, Time of the activity, Total adults, Total children (If applicable, leave blank if not.) , Name of the primary client, Phone number"</t>
-  </si>
-  <si>
     <t>Emails_Reservas</t>
   </si>
   <si>
@@ -529,6 +526,24 @@
   </si>
   <si>
     <t>c.datos7@salascala.com</t>
+  </si>
+  <si>
+    <t>booking@t1.viator.com</t>
+  </si>
+  <si>
+    <t>BODEGAS FERRERA S.L</t>
+  </si>
+  <si>
+    <t>B76684992</t>
+  </si>
+  <si>
+    <t>3786 </t>
+  </si>
+  <si>
+    <t>visitas@bodegasferrera.com</t>
+  </si>
+  <si>
+    <t>Date of the activity, Time of the activity, Total adults, Total children (If applicable, leave blank if not.) , Name of the primary client, Phone number</t>
   </si>
 </sst>
 </file>
@@ -539,7 +554,7 @@
     <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;€&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="0000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,6 +600,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -681,7 +703,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -965,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -1036,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -1089,7 +1111,7 @@
         <v>17</v>
       </c>
       <c r="Q2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1164,7 @@
         <v>17</v>
       </c>
       <c r="Q3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,7 +1211,7 @@
         <v>16</v>
       </c>
       <c r="Q4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1236,7 +1258,7 @@
         <v>16</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1288,6 +1310,9 @@
       <c r="P6" t="s">
         <v>17</v>
       </c>
+      <c r="Q6" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2531,14 +2556,38 @@
       <c r="B34" s="9" t="s">
         <v>154</v>
       </c>
+      <c r="D34" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" t="s">
+        <v>164</v>
+      </c>
       <c r="G34" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="H34">
+        <v>45</v>
+      </c>
+      <c r="J34">
+        <v>45</v>
+      </c>
+      <c r="L34">
+        <v>22</v>
+      </c>
+      <c r="M34">
+        <v>0.28039999999999998</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="O34" s="6" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="P34" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="Q34" s="8"/>
     </row>

</xml_diff>